<commit_message>
move faostat extraction files to workflow v2
</commit_message>
<xml_diff>
--- a/scenario_analysis_v2/scenariov2_pipeline.xlsx
+++ b/scenario_analysis_v2/scenariov2_pipeline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="138">
   <si>
     <t>Section</t>
   </si>
@@ -397,6 +397,42 @@
   </si>
   <si>
     <t>downscaled total demand vector for each county in each scenario; downscaled production vector for each county (relative differences in production do not change by scenario)</t>
+  </si>
+  <si>
+    <t>extract_faostat.R</t>
+  </si>
+  <si>
+    <t>extract_fbs.R</t>
+  </si>
+  <si>
+    <t>process raw FAOSTAT data into usable format, averaging the past 5 years of data for all data points</t>
+  </si>
+  <si>
+    <t>process the food balance sheet data from FAOSTAT, averaging the past 5 years of data for all data points</t>
+  </si>
+  <si>
+    <t>files in raw_data/FAOSTAT/31aug2020</t>
+  </si>
+  <si>
+    <t>raw_data/FAOSTAT/31aug2020/FoodBalanceSheets_E_All_Data_(Normalized).csv; raw_data/FAOSTAT/faostat_item_group_lookup.csv</t>
+  </si>
+  <si>
+    <t>raw FAOSTAT production, emissions, land use, trade, and production value CSVs</t>
+  </si>
+  <si>
+    <t>raw food balance sheet CSV; lookup table for FAOSTAT item groups showing which codes are aggregated from other codes</t>
+  </si>
+  <si>
+    <t>faostat2017/(many files).csv</t>
+  </si>
+  <si>
+    <t>fao_fbs/fbs_*.csv</t>
+  </si>
+  <si>
+    <t>Processed FAOSTAT data files</t>
+  </si>
+  <si>
+    <t>Processed FAOSTAT food balance sheet data files</t>
   </si>
 </sst>
 </file>
@@ -1207,13 +1243,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,7 +1654,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -1626,25 +1662,25 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>79</v>
+        <v>132</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -1652,25 +1688,25 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>83</v>
+        <v>131</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>85</v>
+        <v>133</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -1678,22 +1714,22 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1704,53 +1740,77 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -1758,13 +1818,13 @@
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -1772,6 +1832,34 @@
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Spatial processing pipeline all inside V2
</commit_message>
<xml_diff>
--- a/scenario_analysis_v2/scenariov2_pipeline.xlsx
+++ b/scenario_analysis_v2/scenariov2_pipeline.xlsx
@@ -63,12 +63,6 @@
     <t>Use the county-level weightings to downscale state-level production of goods to the county level, based on numbers of establishments in each county</t>
   </si>
   <si>
-    <t>receipts_bea_sctg_x_state.csv; county_weightings_for_downscale.csv</t>
-  </si>
-  <si>
-    <t>Production by BEA code by state (created in sctg_to_bea.R); number of establishments and employees by BEA code by county</t>
-  </si>
-  <si>
     <t>county_production2012.csv</t>
   </si>
   <si>
@@ -433,6 +427,12 @@
   </si>
   <si>
     <t>Processed FAOSTAT food balance sheet data files</t>
+  </si>
+  <si>
+    <t>susb_nass_workers_receipts_land_bea.csv; county_weightings_for_downscale.csv</t>
+  </si>
+  <si>
+    <t>Production by BEA code by state; number of establishments and employees by BEA code by county</t>
   </si>
 </sst>
 </file>
@@ -1246,10 +1246,10 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,22 +1298,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -1324,22 +1324,22 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="165" x14ac:dyDescent="0.25">
@@ -1353,22 +1353,22 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1382,16 +1382,16 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -1402,10 +1402,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
@@ -1414,10 +1414,10 @@
         <v>11</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1428,22 +1428,22 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1454,22 +1454,22 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1480,22 +1480,22 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -1506,22 +1506,22 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="165" x14ac:dyDescent="0.25">
@@ -1532,22 +1532,22 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1558,22 +1558,22 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -1584,22 +1584,22 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="255" x14ac:dyDescent="0.25">
@@ -1610,22 +1610,22 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="165" x14ac:dyDescent="0.25">
@@ -1636,231 +1636,231 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional documentation for spatial data
</commit_message>
<xml_diff>
--- a/scenario_analysis_v2/scenariov2_pipeline.xlsx
+++ b/scenario_analysis_v2/scenariov2_pipeline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="144">
   <si>
     <t>Section</t>
   </si>
@@ -433,6 +433,24 @@
   </si>
   <si>
     <t>Production by BEA code by state; number of establishments and employees by BEA code by county</t>
+  </si>
+  <si>
+    <t>spatial processing</t>
+  </si>
+  <si>
+    <t>spatial/spatial_processing.Rmd</t>
+  </si>
+  <si>
+    <t>Code notebook combining several scripts. All vector and raster files are transformed to appropriate projections. Intersect TNC ecoregions with both countries and counties. Summarize pixel counts of NLCD and population by TNC-county intersect, and counts of global crop and pasture rasters by TNC-country intersect.</t>
+  </si>
+  <si>
+    <t>Listed in spatial_data.xlsx</t>
+  </si>
+  <si>
+    <t>GPKG files for later plotting (not listed here), CSV files with summary data on NLCD crop and pastureland, USA population, and global crop and pastureland</t>
+  </si>
+  <si>
+    <t>NLCDcrop_county_x_TNC.csv; population_county_x_TNC_longform.csv; global_count_cropdominance.csv; global_count_pasture.csv</t>
   </si>
 </sst>
 </file>
@@ -1243,13 +1261,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,446 +1308,446 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>138</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>109</v>
+        <v>140</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>108</v>
+        <v>141</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>122</v>
+        <v>46</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>72</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>72</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>77</v>
+        <v>131</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1737,129 +1755,155 @@
         <v>72</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>72</v>
       </c>
       <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22">
         <v>20</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>97</v>
       </c>
       <c r="B23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>97</v>
       </c>
       <c r="B24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>97</v>
       </c>
       <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26">
         <v>24</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create data sources table Include even more raw data processing scripts into standalone pipeline
</commit_message>
<xml_diff>
--- a/scenario_analysis_v2/scenariov2_pipeline.xlsx
+++ b/scenario_analysis_v2/scenariov2_pipeline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="163">
   <si>
     <t>Section</t>
   </si>
@@ -159,9 +159,6 @@
     <t>First use the county-level personal income data to downscale the BEA baseline personal consumption expenditures vector to each county. Then, use the consumption factors to create an alternative vector for each county in each scenario. Next, apply the I-O approach by multiplying the Leontief inverse by the vector for each county to get the total demand from each county in each scenario, including intermediate.</t>
   </si>
   <si>
-    <t>data/raw_data/commodity_flows/Lin_supp_info/County Personal Income.xlsx; data/raw_data/BEA/formatted/use2012.csv; USEEIO2012_DRC.csv; bea_consumption_factors_diet_waste_scenarios.csv</t>
-  </si>
-  <si>
     <t>Total personal income for each USA county in 2012; use table from the 2012 BEA data; direct requirements coefficient matrix from the built USEEIO model; food consumption factors by BEA code for all scenarios</t>
   </si>
   <si>
@@ -451,6 +448,66 @@
   </si>
   <si>
     <t>NLCDcrop_county_x_TNC.csv; population_county_x_TNC_longform.csv; global_count_cropdominance.csv; global_count_pasture.csv</t>
+  </si>
+  <si>
+    <t>raw_data/commodity_flows/Lin_supp_info/County Personal Income.xlsx; useeio2012v2.0_pce_drc.RData; bea_consumption_factors_diet_waste_scenarios.csv</t>
+  </si>
+  <si>
+    <t>read_clean_lafa_data.R</t>
+  </si>
+  <si>
+    <t>data/raw_data/USDA/LAFA/*.xls</t>
+  </si>
+  <si>
+    <t>Raw LAFA data</t>
+  </si>
+  <si>
+    <t>lafa_cleaned.csv</t>
+  </si>
+  <si>
+    <t>read_chaudh2018_si.R</t>
+  </si>
+  <si>
+    <t>Convert supplementary information from Chaudhary and Brooks 2018 (biodiversity characterization factors) to clean form</t>
+  </si>
+  <si>
+    <t>raw_data/biodiversity/chaudhary2015SI/chaudhary_brooks_2018_si.xlsx</t>
+  </si>
+  <si>
+    <t>Raw supplemental file from Chaudhary and Brooks</t>
+  </si>
+  <si>
+    <t>raw_data/biodiversity/chaudhary2015SI/chaud2018si_CFs.csv</t>
+  </si>
+  <si>
+    <t>Cleaned LAFA data for the most recent year, in a single CSV</t>
+  </si>
+  <si>
+    <t>Cleaned biodiversity characterization factors in a single CSV</t>
+  </si>
+  <si>
+    <t>data pre-processing</t>
+  </si>
+  <si>
+    <t>read_qfahpd_data.R</t>
+  </si>
+  <si>
+    <t>Convert raw LAFA data to a single data frame and write to CSV</t>
+  </si>
+  <si>
+    <t>Convert raw QFAHPD data to a single data frame and write to CSV</t>
+  </si>
+  <si>
+    <t>raw_data/USDA/QFAHPD/*.xls</t>
+  </si>
+  <si>
+    <t>Raw QFAHPD data</t>
+  </si>
+  <si>
+    <t>QFAHPD/tidy_data/qfahpd2.csv</t>
+  </si>
+  <si>
+    <t>Cleaned QFAHPD version 2 data, in a single CSV</t>
   </si>
 </sst>
 </file>
@@ -1261,13 +1318,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,184 +1367,184 @@
     </row>
     <row r="2" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>155</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -1495,103 +1552,103 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>29</v>
+        <v>136</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -1599,312 +1656,390 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>122</v>
+        <v>34</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>123</v>
+        <v>35</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H16" s="1" t="s">
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17">
-        <v>15</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19">
-        <v>17</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20">
-        <v>18</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>89</v>
+        <v>130</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B22">
-        <v>20</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F25" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H25" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H22" s="1" t="s">
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B23">
-        <v>21</v>
-      </c>
-      <c r="C23" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="1" t="s">
+    </row>
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24">
-        <v>22</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="1" t="s">
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25">
-        <v>23</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="1" t="s">
+    </row>
+    <row r="29" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26">
-        <v>24</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>